<commit_message>
final objective and manager
</commit_message>
<xml_diff>
--- a/data scraping/combined_data - Copy full.xlsx
+++ b/data scraping/combined_data - Copy full.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Staging\data scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E28F567-3B73-406E-B39B-3FDC23573AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDEDB06-5A22-4916-ACF9-CEB3793EFC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="12" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="31" activeTab="33" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Icici Prudential Value Discover" sheetId="1" r:id="rId1"/>
@@ -22713,7 +22713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:CA38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0"/>
+    <sheetView topLeftCell="AR1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -33809,7 +33809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:BG38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="N1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -43753,7 +43753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:CC38"/>
   <sheetViews>
-    <sheetView topLeftCell="BP1" workbookViewId="0"/>
+    <sheetView topLeftCell="AY1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -47344,7 +47344,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:CA38"/>
   <sheetViews>
-    <sheetView topLeftCell="BX1" workbookViewId="0"/>
+    <sheetView topLeftCell="BH1" workbookViewId="0">
+      <selection activeCell="BS29" sqref="BS29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -51013,9 +51015,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:BG38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="50.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="38" width="7" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="50.88671875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="6" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="5" bestFit="1" customWidth="1"/>
+    <col min="46" max="51" width="7" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="6" bestFit="1" customWidth="1"/>
+    <col min="55" max="56" width="5" bestFit="1" customWidth="1"/>
+    <col min="57" max="58" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="25.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">

</xml_diff>